<commit_message>
trying in mixed effects
</commit_message>
<xml_diff>
--- a/Sebjan_dp_new.xlsx
+++ b/Sebjan_dp_new.xlsx
@@ -511,10 +511,10 @@
     <t>L-pl-adj</t>
   </si>
   <si>
-    <t>kIč-nr-n</t>
+    <t>REkEn-iter.adv-num</t>
   </si>
   <si>
-    <t>REkEn-iter.adv-num</t>
+    <t>kIč-nr-n</t>
   </si>
   <si>
     <t>nrI-2sg-aux</t>
@@ -757,10 +757,10 @@
     <t>Č-res-v</t>
   </si>
   <si>
-    <t>nIkEn-sim.cvb-v</t>
+    <t>DEŋ-pst.ptc-v</t>
   </si>
   <si>
-    <t>DEŋ-pst.ptc-v</t>
+    <t>nIkEn-sim.cvb-v</t>
   </si>
   <si>
     <t>RIdʒI-ant.cvb-v</t>
@@ -1323,7 +1323,7 @@
     </row>
     <row r="2" spans="1:56">
       <c r="A2" s="1">
-        <v>309</v>
+        <v>628</v>
       </c>
       <c r="B2" t="s">
         <v>55</v>
@@ -1332,7 +1332,7 @@
         <v>66</v>
       </c>
       <c r="D2">
-        <v>0.505746622855057</v>
+        <v>0.505766703176342</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="3" spans="1:56">
       <c r="A3" s="1">
-        <v>356</v>
+        <v>599</v>
       </c>
       <c r="B3" t="s">
         <v>56</v>
@@ -1502,7 +1502,7 @@
         <v>19</v>
       </c>
       <c r="D3">
-        <v>0.47892464595223</v>
+        <v>0.478944726273515</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="4" spans="1:56">
       <c r="A4" s="1">
-        <v>525</v>
+        <v>654</v>
       </c>
       <c r="B4" t="s">
         <v>57</v>
@@ -1672,7 +1672,7 @@
         <v>30</v>
       </c>
       <c r="D4">
-        <v>0.457781124497992</v>
+        <v>0.457801204819277</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="5" spans="1:56">
       <c r="A5" s="1">
-        <v>56</v>
+        <v>497</v>
       </c>
       <c r="B5" t="s">
         <v>58</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="6" spans="1:56">
       <c r="A6" s="1">
-        <v>643</v>
+        <v>353</v>
       </c>
       <c r="B6" t="s">
         <v>59</v>
@@ -2173,7 +2173,7 @@
     </row>
     <row r="7" spans="1:56">
       <c r="A7" s="1">
-        <v>358</v>
+        <v>393</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
@@ -2182,7 +2182,7 @@
         <v>30</v>
       </c>
       <c r="D7">
-        <v>0.440612449799197</v>
+        <v>0.440632530120482</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="8" spans="1:56">
       <c r="A8" s="1">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>61</v>
@@ -2513,7 +2513,7 @@
     </row>
     <row r="9" spans="1:56">
       <c r="A9" s="1">
-        <v>270</v>
+        <v>378</v>
       </c>
       <c r="B9" t="s">
         <v>62</v>
@@ -2522,7 +2522,7 @@
         <v>53</v>
       </c>
       <c r="D9">
-        <v>0.421782223232553</v>
+        <v>0.421802303553838</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2683,7 +2683,7 @@
     </row>
     <row r="10" spans="1:56">
       <c r="A10" s="1">
-        <v>247</v>
+        <v>359</v>
       </c>
       <c r="B10" t="s">
         <v>63</v>
@@ -2692,7 +2692,7 @@
         <v>88</v>
       </c>
       <c r="D10">
-        <v>0.41504016064257</v>
+        <v>0.415070281124498</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2853,7 +2853,7 @@
     </row>
     <row r="11" spans="1:56">
       <c r="A11" s="1">
-        <v>668</v>
+        <v>285</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
@@ -2862,7 +2862,7 @@
         <v>19</v>
       </c>
       <c r="D11">
-        <v>0.414647537518495</v>
+        <v>0.41466761783978</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -3023,7 +3023,7 @@
     </row>
     <row r="12" spans="1:56">
       <c r="A12" s="1">
-        <v>445</v>
+        <v>534</v>
       </c>
       <c r="B12" t="s">
         <v>65</v>
@@ -3032,7 +3032,7 @@
         <v>47</v>
       </c>
       <c r="D12">
-        <v>0.393719986328292</v>
+        <v>0.393730026488934</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -3193,7 +3193,7 @@
     </row>
     <row r="13" spans="1:56">
       <c r="A13" s="1">
-        <v>621</v>
+        <v>371</v>
       </c>
       <c r="B13" t="s">
         <v>66</v>
@@ -3363,7 +3363,7 @@
     </row>
     <row r="14" spans="1:56">
       <c r="A14" s="1">
-        <v>390</v>
+        <v>609</v>
       </c>
       <c r="B14" t="s">
         <v>67</v>
@@ -3533,7 +3533,7 @@
     </row>
     <row r="15" spans="1:56">
       <c r="A15" s="1">
-        <v>655</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
         <v>68</v>
@@ -3703,7 +3703,7 @@
     </row>
     <row r="16" spans="1:56">
       <c r="A16" s="1">
-        <v>168</v>
+        <v>597</v>
       </c>
       <c r="B16" t="s">
         <v>69</v>
@@ -3712,7 +3712,7 @@
         <v>52</v>
       </c>
       <c r="D16">
-        <v>0.382184893419833</v>
+        <v>0.382204973741118</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -3873,7 +3873,7 @@
     </row>
     <row r="17" spans="1:56">
       <c r="A17" s="1">
-        <v>556</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s">
         <v>70</v>
@@ -4043,7 +4043,7 @@
     </row>
     <row r="18" spans="1:56">
       <c r="A18" s="1">
-        <v>408</v>
+        <v>601</v>
       </c>
       <c r="B18" t="s">
         <v>71</v>
@@ -4052,7 +4052,7 @@
         <v>59</v>
       </c>
       <c r="D18">
-        <v>0.379158498400381</v>
+        <v>0.379178578721666</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -4213,7 +4213,7 @@
     </row>
     <row r="19" spans="1:56">
       <c r="A19" s="1">
-        <v>366</v>
+        <v>607</v>
       </c>
       <c r="B19" t="s">
         <v>72</v>
@@ -4222,7 +4222,7 @@
         <v>28</v>
       </c>
       <c r="D19">
-        <v>0.377923121055651</v>
+        <v>0.377943201376936</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -4383,7 +4383,7 @@
     </row>
     <row r="20" spans="1:56">
       <c r="A20" s="1">
-        <v>633</v>
+        <v>553</v>
       </c>
       <c r="B20" t="s">
         <v>73</v>
@@ -4392,7 +4392,7 @@
         <v>22</v>
       </c>
       <c r="D20">
-        <v>0.371560788608981</v>
+        <v>0.371570828769624</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -4553,7 +4553,7 @@
     </row>
     <row r="21" spans="1:56">
       <c r="A21" s="1">
-        <v>360</v>
+        <v>284</v>
       </c>
       <c r="B21" t="s">
         <v>74</v>
@@ -4723,7 +4723,7 @@
     </row>
     <row r="22" spans="1:56">
       <c r="A22" s="1">
-        <v>431</v>
+        <v>551</v>
       </c>
       <c r="B22" t="s">
         <v>75</v>
@@ -4893,7 +4893,7 @@
     </row>
     <row r="23" spans="1:56">
       <c r="A23" s="1">
-        <v>259</v>
+        <v>333</v>
       </c>
       <c r="B23" t="s">
         <v>76</v>
@@ -4902,7 +4902,7 @@
         <v>27</v>
       </c>
       <c r="D23">
-        <v>0.365083668005355</v>
+        <v>0.365093708165997</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -5063,7 +5063,7 @@
     </row>
     <row r="24" spans="1:56">
       <c r="A24" s="1">
-        <v>138</v>
+        <v>656</v>
       </c>
       <c r="B24" t="s">
         <v>77</v>
@@ -5233,7 +5233,7 @@
     </row>
     <row r="25" spans="1:56">
       <c r="A25" s="1">
-        <v>77</v>
+        <v>288</v>
       </c>
       <c r="B25" t="s">
         <v>78</v>
@@ -5242,7 +5242,7 @@
         <v>70</v>
       </c>
       <c r="D25">
-        <v>0.363674698795181</v>
+        <v>0.363664658634538</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -5403,7 +5403,7 @@
     </row>
     <row r="26" spans="1:56">
       <c r="A26" s="1">
-        <v>663</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
         <v>79</v>
@@ -5412,7 +5412,7 @@
         <v>19</v>
       </c>
       <c r="D26">
-        <v>0.361656626506024</v>
+        <v>0.361676706827309</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -5573,7 +5573,7 @@
     </row>
     <row r="27" spans="1:56">
       <c r="A27" s="1">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="B27" t="s">
         <v>80</v>
@@ -5582,7 +5582,7 @@
         <v>73</v>
       </c>
       <c r="D27">
-        <v>0.3598789679265</v>
+        <v>0.359899048247786</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -5743,7 +5743,7 @@
     </row>
     <row r="28" spans="1:56">
       <c r="A28" s="1">
-        <v>111</v>
+        <v>450</v>
       </c>
       <c r="B28" t="s">
         <v>81</v>
@@ -5752,7 +5752,7 @@
         <v>39</v>
       </c>
       <c r="D28">
-        <v>0.357768767377201</v>
+        <v>0.357798887859129</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -5913,7 +5913,7 @@
     </row>
     <row r="29" spans="1:56">
       <c r="A29" s="1">
-        <v>117</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
         <v>82</v>
@@ -5922,7 +5922,7 @@
         <v>34</v>
       </c>
       <c r="D29">
-        <v>0.357111977321049</v>
+        <v>0.357122017481692</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -6083,7 +6083,7 @@
     </row>
     <row r="30" spans="1:56">
       <c r="A30" s="1">
-        <v>637</v>
+        <v>175</v>
       </c>
       <c r="B30" t="s">
         <v>83</v>
@@ -6253,7 +6253,7 @@
     </row>
     <row r="31" spans="1:56">
       <c r="A31" s="1">
-        <v>129</v>
+        <v>229</v>
       </c>
       <c r="B31" t="s">
         <v>84</v>
@@ -6262,7 +6262,7 @@
         <v>845</v>
       </c>
       <c r="D31">
-        <v>0.356046374848506</v>
+        <v>0.356016254366579</v>
       </c>
       <c r="E31">
         <v>0.00118343195266272</v>
@@ -6423,7 +6423,7 @@
     </row>
     <row r="32" spans="1:56">
       <c r="A32" s="1">
-        <v>495</v>
+        <v>134</v>
       </c>
       <c r="B32" t="s">
         <v>85</v>
@@ -6432,7 +6432,7 @@
         <v>53</v>
       </c>
       <c r="D32">
-        <v>0.354157005380011</v>
+        <v>0.354167045540653</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -6593,7 +6593,7 @@
     </row>
     <row r="33" spans="1:56">
       <c r="A33" s="1">
-        <v>531</v>
+        <v>344</v>
       </c>
       <c r="B33" t="s">
         <v>86</v>
@@ -6602,7 +6602,7 @@
         <v>36</v>
       </c>
       <c r="D33">
-        <v>0.352951807228916</v>
+        <v>0.352971887550201</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -6763,7 +6763,7 @@
     </row>
     <row r="34" spans="1:56">
       <c r="A34" s="1">
-        <v>478</v>
+        <v>412</v>
       </c>
       <c r="B34" t="s">
         <v>87</v>
@@ -6772,7 +6772,7 @@
         <v>66</v>
       </c>
       <c r="D34">
-        <v>0.352405074844834</v>
+        <v>0.352415115005476</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -6933,7 +6933,7 @@
     </row>
     <row r="35" spans="1:56">
       <c r="A35" s="1">
-        <v>403</v>
+        <v>322</v>
       </c>
       <c r="B35" t="s">
         <v>88</v>
@@ -7103,7 +7103,7 @@
     </row>
     <row r="36" spans="1:56">
       <c r="A36" s="1">
-        <v>197</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
         <v>89</v>
@@ -7273,7 +7273,7 @@
     </row>
     <row r="37" spans="1:56">
       <c r="A37" s="1">
-        <v>667</v>
+        <v>118</v>
       </c>
       <c r="B37" t="s">
         <v>90</v>
@@ -7443,7 +7443,7 @@
     </row>
     <row r="38" spans="1:56">
       <c r="A38" s="1">
-        <v>410</v>
+        <v>281</v>
       </c>
       <c r="B38" t="s">
         <v>91</v>
@@ -7452,7 +7452,7 @@
         <v>20</v>
       </c>
       <c r="D38">
-        <v>0.344417670682731</v>
+        <v>0.344437751004016</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -7613,7 +7613,7 @@
     </row>
     <row r="39" spans="1:56">
       <c r="A39" s="1">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="B39" t="s">
         <v>92</v>
@@ -7622,7 +7622,7 @@
         <v>1895</v>
       </c>
       <c r="D39">
-        <v>0.343905595998771</v>
+        <v>0.343875475516843</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -7783,7 +7783,7 @@
     </row>
     <row r="40" spans="1:56">
       <c r="A40" s="1">
-        <v>222</v>
+        <v>411</v>
       </c>
       <c r="B40" t="s">
         <v>93</v>
@@ -7792,7 +7792,7 @@
         <v>37</v>
       </c>
       <c r="D40">
-        <v>0.34379952241398</v>
+        <v>0.343819602735265</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -7953,7 +7953,7 @@
     </row>
     <row r="41" spans="1:56">
       <c r="A41" s="1">
-        <v>2</v>
+        <v>516</v>
       </c>
       <c r="B41" t="s">
         <v>94</v>
@@ -8123,7 +8123,7 @@
     </row>
     <row r="42" spans="1:56">
       <c r="A42" s="1">
-        <v>214</v>
+        <v>386</v>
       </c>
       <c r="B42" t="s">
         <v>95</v>
@@ -8132,7 +8132,7 @@
         <v>45</v>
       </c>
       <c r="D42">
-        <v>0.342751004016064</v>
+        <v>0.342781124497992</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -8293,7 +8293,7 @@
     </row>
     <row r="43" spans="1:56">
       <c r="A43" s="1">
-        <v>588</v>
+        <v>667</v>
       </c>
       <c r="B43" t="s">
         <v>96</v>
@@ -8463,7 +8463,7 @@
     </row>
     <row r="44" spans="1:56">
       <c r="A44" s="1">
-        <v>465</v>
+        <v>614</v>
       </c>
       <c r="B44" t="s">
         <v>97</v>
@@ -8472,7 +8472,7 @@
         <v>16</v>
       </c>
       <c r="D44">
-        <v>0.340220883534137</v>
+        <v>0.340220883534136</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -8633,7 +8633,7 @@
     </row>
     <row r="45" spans="1:56">
       <c r="A45" s="1">
-        <v>509</v>
+        <v>421</v>
       </c>
       <c r="B45" t="s">
         <v>98</v>
@@ -8803,7 +8803,7 @@
     </row>
     <row r="46" spans="1:56">
       <c r="A46" s="1">
-        <v>290</v>
+        <v>608</v>
       </c>
       <c r="B46" t="s">
         <v>99</v>
@@ -8973,7 +8973,7 @@
     </row>
     <row r="47" spans="1:56">
       <c r="A47" s="1">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="B47" t="s">
         <v>100</v>
@@ -9143,7 +9143,7 @@
     </row>
     <row r="48" spans="1:56">
       <c r="A48" s="1">
-        <v>17</v>
+        <v>366</v>
       </c>
       <c r="B48" t="s">
         <v>101</v>
@@ -9152,7 +9152,7 @@
         <v>21</v>
       </c>
       <c r="D48">
-        <v>0.335352839931153</v>
+        <v>0.335362880091796</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -9313,7 +9313,7 @@
     </row>
     <row r="49" spans="1:56">
       <c r="A49" s="1">
-        <v>589</v>
+        <v>558</v>
       </c>
       <c r="B49" t="s">
         <v>102</v>
@@ -9483,7 +9483,7 @@
     </row>
     <row r="50" spans="1:56">
       <c r="A50" s="1">
-        <v>134</v>
+        <v>256</v>
       </c>
       <c r="B50" t="s">
         <v>103</v>
@@ -9492,7 +9492,7 @@
         <v>44</v>
       </c>
       <c r="D50">
-        <v>0.331916757940854</v>
+        <v>0.331936838262139</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -9653,7 +9653,7 @@
     </row>
     <row r="51" spans="1:56">
       <c r="A51" s="1">
-        <v>9</v>
+        <v>167</v>
       </c>
       <c r="B51" t="s">
         <v>104</v>
@@ -9823,7 +9823,7 @@
     </row>
     <row r="52" spans="1:56">
       <c r="A52" s="1">
-        <v>115</v>
+        <v>644</v>
       </c>
       <c r="B52" t="s">
         <v>105</v>
@@ -9993,7 +9993,7 @@
     </row>
     <row r="53" spans="1:56">
       <c r="A53" s="1">
-        <v>128</v>
+        <v>420</v>
       </c>
       <c r="B53" t="s">
         <v>106</v>
@@ -10002,7 +10002,7 @@
         <v>106</v>
       </c>
       <c r="D53">
-        <v>0.327224369174812</v>
+        <v>0.327194248692885</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -10163,7 +10163,7 @@
     </row>
     <row r="54" spans="1:56">
       <c r="A54" s="1">
-        <v>155</v>
+        <v>418</v>
       </c>
       <c r="B54" t="s">
         <v>107</v>
@@ -10172,7 +10172,7 @@
         <v>24</v>
       </c>
       <c r="D54">
-        <v>0.326646586345382</v>
+        <v>0.326676706827309</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -10333,7 +10333,7 @@
     </row>
     <row r="55" spans="1:56">
       <c r="A55" s="1">
-        <v>184</v>
+        <v>235</v>
       </c>
       <c r="B55" t="s">
         <v>108</v>
@@ -10342,7 +10342,7 @@
         <v>263</v>
       </c>
       <c r="D55">
-        <v>0.326204399346435</v>
+        <v>0.32622447966772</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -10503,7 +10503,7 @@
     </row>
     <row r="56" spans="1:56">
       <c r="A56" s="1">
-        <v>405</v>
+        <v>136</v>
       </c>
       <c r="B56" t="s">
         <v>109</v>
@@ -10512,7 +10512,7 @@
         <v>94</v>
       </c>
       <c r="D56">
-        <v>0.325769460822011</v>
+        <v>0.325779500982654</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -10673,7 +10673,7 @@
     </row>
     <row r="57" spans="1:56">
       <c r="A57" s="1">
-        <v>146</v>
+        <v>297</v>
       </c>
       <c r="B57" t="s">
         <v>110</v>
@@ -10682,7 +10682,7 @@
         <v>17</v>
       </c>
       <c r="D57">
-        <v>0.325353177415545</v>
+        <v>0.32537325773683</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -10843,7 +10843,7 @@
     </row>
     <row r="58" spans="1:56">
       <c r="A58" s="1">
-        <v>242</v>
+        <v>589</v>
       </c>
       <c r="B58" t="s">
         <v>111</v>
@@ -10852,7 +10852,7 @@
         <v>425</v>
       </c>
       <c r="D58">
-        <v>0.32479447200567</v>
+        <v>0.324804512166312</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -11013,7 +11013,7 @@
     </row>
     <row r="59" spans="1:56">
       <c r="A59" s="1">
-        <v>114</v>
+        <v>358</v>
       </c>
       <c r="B59" t="s">
         <v>112</v>
@@ -11022,7 +11022,7 @@
         <v>127</v>
       </c>
       <c r="D59">
-        <v>0.324507636846599</v>
+        <v>0.324497596685956</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -11183,7 +11183,7 @@
     </row>
     <row r="60" spans="1:56">
       <c r="A60" s="1">
-        <v>457</v>
+        <v>71</v>
       </c>
       <c r="B60" t="s">
         <v>113</v>
@@ -11192,7 +11192,7 @@
         <v>31</v>
       </c>
       <c r="D60">
-        <v>0.32364846482705</v>
+        <v>0.323658504987693</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -11353,7 +11353,7 @@
     </row>
     <row r="61" spans="1:56">
       <c r="A61" s="1">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B61" t="s">
         <v>114</v>
@@ -11362,7 +11362,7 @@
         <v>25</v>
       </c>
       <c r="D61">
-        <v>0.322941767068273</v>
+        <v>0.322961847389558</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -11523,7 +11523,7 @@
     </row>
     <row r="62" spans="1:56">
       <c r="A62" s="1">
-        <v>68</v>
+        <v>252</v>
       </c>
       <c r="B62" t="s">
         <v>115</v>
@@ -11532,7 +11532,7 @@
         <v>189</v>
       </c>
       <c r="D62">
-        <v>0.32263753426404</v>
+        <v>0.322647574424683</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -11693,7 +11693,7 @@
     </row>
     <row r="63" spans="1:56">
       <c r="A63" s="1">
-        <v>596</v>
+        <v>89</v>
       </c>
       <c r="B63" t="s">
         <v>116</v>
@@ -11702,7 +11702,7 @@
         <v>25</v>
       </c>
       <c r="D63">
-        <v>0.321957831325301</v>
+        <v>0.321977911646586</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -11863,7 +11863,7 @@
     </row>
     <row r="64" spans="1:56">
       <c r="A64" s="1">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="B64" t="s">
         <v>117</v>
@@ -12033,7 +12033,7 @@
     </row>
     <row r="65" spans="1:56">
       <c r="A65" s="1">
-        <v>194</v>
+        <v>573</v>
       </c>
       <c r="B65" t="s">
         <v>118</v>
@@ -12042,7 +12042,7 @@
         <v>216</v>
       </c>
       <c r="D65">
-        <v>0.321035252119589</v>
+        <v>0.321065372601517</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -12203,7 +12203,7 @@
     </row>
     <row r="66" spans="1:56">
       <c r="A66" s="1">
-        <v>319</v>
+        <v>617</v>
       </c>
       <c r="B66" t="s">
         <v>119</v>
@@ -12212,7 +12212,7 @@
         <v>19</v>
       </c>
       <c r="D66">
-        <v>0.319366413020503</v>
+        <v>0.319376453181146</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -12373,7 +12373,7 @@
     </row>
     <row r="67" spans="1:56">
       <c r="A67" s="1">
-        <v>533</v>
+        <v>416</v>
       </c>
       <c r="B67" t="s">
         <v>120</v>
@@ -12543,7 +12543,7 @@
     </row>
     <row r="68" spans="1:56">
       <c r="A68" s="1">
-        <v>268</v>
+        <v>148</v>
       </c>
       <c r="B68" t="s">
         <v>121</v>
@@ -12552,7 +12552,7 @@
         <v>22</v>
       </c>
       <c r="D68">
-        <v>0.31886272362176</v>
+        <v>0.318892844103687</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -12713,7 +12713,7 @@
     </row>
     <row r="69" spans="1:56">
       <c r="A69" s="1">
-        <v>419</v>
+        <v>302</v>
       </c>
       <c r="B69" t="s">
         <v>122</v>
@@ -12722,7 +12722,7 @@
         <v>36</v>
       </c>
       <c r="D69">
-        <v>0.318165997322624</v>
+        <v>0.318176037483266</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -12883,7 +12883,7 @@
     </row>
     <row r="70" spans="1:56">
       <c r="A70" s="1">
-        <v>595</v>
+        <v>577</v>
       </c>
       <c r="B70" t="s">
         <v>123</v>
@@ -12892,7 +12892,7 @@
         <v>80</v>
       </c>
       <c r="D70">
-        <v>0.318032128514056</v>
+        <v>0.318022088353414</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -13053,7 +13053,7 @@
     </row>
     <row r="71" spans="1:56">
       <c r="A71" s="1">
-        <v>224</v>
+        <v>598</v>
       </c>
       <c r="B71" t="s">
         <v>124</v>
@@ -13223,7 +13223,7 @@
     </row>
     <row r="72" spans="1:56">
       <c r="A72" s="1">
-        <v>131</v>
+        <v>301</v>
       </c>
       <c r="B72" t="s">
         <v>125</v>
@@ -13393,7 +13393,7 @@
     </row>
     <row r="73" spans="1:56">
       <c r="A73" s="1">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B73" t="s">
         <v>126</v>
@@ -13563,7 +13563,7 @@
     </row>
     <row r="74" spans="1:56">
       <c r="A74" s="1">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="B74" t="s">
         <v>127</v>
@@ -13572,7 +13572,7 @@
         <v>35</v>
       </c>
       <c r="D74">
-        <v>0.314958405048766</v>
+        <v>0.314968445209409</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -13733,7 +13733,7 @@
     </row>
     <row r="75" spans="1:56">
       <c r="A75" s="1">
-        <v>212</v>
+        <v>352</v>
       </c>
       <c r="B75" t="s">
         <v>128</v>
@@ -13742,7 +13742,7 @@
         <v>53</v>
       </c>
       <c r="D75">
-        <v>0.314606728802</v>
+        <v>0.314616768962643</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -13903,7 +13903,7 @@
     </row>
     <row r="76" spans="1:56">
       <c r="A76" s="1">
-        <v>448</v>
+        <v>114</v>
       </c>
       <c r="B76" t="s">
         <v>129</v>
@@ -13912,7 +13912,7 @@
         <v>18</v>
       </c>
       <c r="D76">
-        <v>0.313396921017403</v>
+        <v>0.313427041499331</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -14073,7 +14073,7 @@
     </row>
     <row r="77" spans="1:56">
       <c r="A77" s="1">
-        <v>271</v>
+        <v>181</v>
       </c>
       <c r="B77" t="s">
         <v>130</v>
@@ -14082,7 +14082,7 @@
         <v>122</v>
       </c>
       <c r="D77">
-        <v>0.312724010797288</v>
+        <v>0.312754131279215</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -14243,7 +14243,7 @@
     </row>
     <row r="78" spans="1:56">
       <c r="A78" s="1">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B78" t="s">
         <v>131</v>
@@ -14252,7 +14252,7 @@
         <v>45</v>
       </c>
       <c r="D78">
-        <v>0.310826639892905</v>
+        <v>0.310816599732262</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -14413,7 +14413,7 @@
     </row>
     <row r="79" spans="1:56">
       <c r="A79" s="1">
-        <v>276</v>
+        <v>430</v>
       </c>
       <c r="B79" t="s">
         <v>132</v>
@@ -14592,7 +14592,7 @@
         <v>23</v>
       </c>
       <c r="D80">
-        <v>0.309681334031779</v>
+        <v>0.309691374192422</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -14753,7 +14753,7 @@
     </row>
     <row r="81" spans="1:56">
       <c r="A81" s="1">
-        <v>561</v>
+        <v>395</v>
       </c>
       <c r="B81" t="s">
         <v>134</v>
@@ -14762,7 +14762,7 @@
         <v>110</v>
       </c>
       <c r="D81">
-        <v>0.309611171960569</v>
+        <v>0.309621212121212</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -14923,7 +14923,7 @@
     </row>
     <row r="82" spans="1:56">
       <c r="A82" s="1">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="B82" t="s">
         <v>135</v>
@@ -14932,7 +14932,7 @@
         <v>61</v>
       </c>
       <c r="D82">
-        <v>0.309533708604911</v>
+        <v>0.309543748765554</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -15093,7 +15093,7 @@
     </row>
     <row r="83" spans="1:56">
       <c r="A83" s="1">
-        <v>411</v>
+        <v>370</v>
       </c>
       <c r="B83" t="s">
         <v>136</v>
@@ -15102,7 +15102,7 @@
         <v>49</v>
       </c>
       <c r="D83">
-        <v>0.307684616015081</v>
+        <v>0.307694656175723</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -15263,7 +15263,7 @@
     </row>
     <row r="84" spans="1:56">
       <c r="A84" s="1">
-        <v>84</v>
+        <v>179</v>
       </c>
       <c r="B84" t="s">
         <v>137</v>
@@ -15433,7 +15433,7 @@
     </row>
     <row r="85" spans="1:56">
       <c r="A85" s="1">
-        <v>359</v>
+        <v>72</v>
       </c>
       <c r="B85" t="s">
         <v>138</v>
@@ -15442,7 +15442,7 @@
         <v>19</v>
       </c>
       <c r="D85">
-        <v>0.305099344747411</v>
+        <v>0.305129465229338</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -15603,7 +15603,7 @@
     </row>
     <row r="86" spans="1:56">
       <c r="A86" s="1">
-        <v>399</v>
+        <v>634</v>
       </c>
       <c r="B86" t="s">
         <v>139</v>
@@ -15612,7 +15612,7 @@
         <v>60</v>
       </c>
       <c r="D86">
-        <v>0.304859437751004</v>
+        <v>0.304849397590361</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -15773,7 +15773,7 @@
     </row>
     <row r="87" spans="1:56">
       <c r="A87" s="1">
-        <v>485</v>
+        <v>168</v>
       </c>
       <c r="B87" t="s">
         <v>140</v>
@@ -15943,7 +15943,7 @@
     </row>
     <row r="88" spans="1:56">
       <c r="A88" s="1">
-        <v>18</v>
+        <v>541</v>
       </c>
       <c r="B88" t="s">
         <v>141</v>
@@ -15952,7 +15952,7 @@
         <v>16</v>
       </c>
       <c r="D88">
-        <v>0.303293172690763</v>
+        <v>0.303313253012048</v>
       </c>
       <c r="E88">
         <v>0</v>
@@ -16113,7 +16113,7 @@
     </row>
     <row r="89" spans="1:56">
       <c r="A89" s="1">
-        <v>656</v>
+        <v>99</v>
       </c>
       <c r="B89" t="s">
         <v>142</v>
@@ -16122,7 +16122,7 @@
         <v>132</v>
       </c>
       <c r="D89">
-        <v>0.302718145308507</v>
+        <v>0.302698064987222</v>
       </c>
       <c r="E89">
         <v>0</v>
@@ -16283,7 +16283,7 @@
     </row>
     <row r="90" spans="1:56">
       <c r="A90" s="1">
-        <v>534</v>
+        <v>340</v>
       </c>
       <c r="B90" t="s">
         <v>143</v>
@@ -16292,7 +16292,7 @@
         <v>61</v>
       </c>
       <c r="D90">
-        <v>0.302078148660215</v>
+        <v>0.302108269142142</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -16453,7 +16453,7 @@
     </row>
     <row r="91" spans="1:56">
       <c r="A91" s="1">
-        <v>474</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
         <v>144</v>
@@ -16462,7 +16462,7 @@
         <v>19</v>
       </c>
       <c r="D91">
-        <v>0.300902557598816</v>
+        <v>0.300912597759459</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -16623,7 +16623,7 @@
     </row>
     <row r="92" spans="1:56">
       <c r="A92" s="1">
-        <v>315</v>
+        <v>533</v>
       </c>
       <c r="B92" t="s">
         <v>145</v>
@@ -16793,7 +16793,7 @@
     </row>
     <row r="93" spans="1:56">
       <c r="A93" s="1">
-        <v>552</v>
+        <v>190</v>
       </c>
       <c r="B93" t="s">
         <v>146</v>
@@ -16802,7 +16802,7 @@
         <v>46</v>
       </c>
       <c r="D93">
-        <v>0.30006198707875</v>
+        <v>0.300092107560677</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -16963,7 +16963,7 @@
     </row>
     <row r="94" spans="1:56">
       <c r="A94" s="1">
-        <v>583</v>
+        <v>549</v>
       </c>
       <c r="B94" t="s">
         <v>147</v>
@@ -16972,7 +16972,7 @@
         <v>18</v>
       </c>
       <c r="D94">
-        <v>0.299675368139224</v>
+        <v>0.299695448460509</v>
       </c>
       <c r="E94">
         <v>0</v>
@@ -17133,7 +17133,7 @@
     </row>
     <row r="95" spans="1:56">
       <c r="A95" s="1">
-        <v>341</v>
+        <v>518</v>
       </c>
       <c r="B95" t="s">
         <v>148</v>
@@ -17142,7 +17142,7 @@
         <v>57</v>
       </c>
       <c r="D95">
-        <v>0.298281547241598</v>
+        <v>0.298301627562883</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -17303,7 +17303,7 @@
     </row>
     <row r="96" spans="1:56">
       <c r="A96" s="1">
-        <v>492</v>
+        <v>310</v>
       </c>
       <c r="B96" t="s">
         <v>149</v>
@@ -17312,7 +17312,7 @@
         <v>340</v>
       </c>
       <c r="D96">
-        <v>0.297567918733759</v>
+        <v>0.297537798251831</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -17473,7 +17473,7 @@
     </row>
     <row r="97" spans="1:56">
       <c r="A97" s="1">
-        <v>286</v>
+        <v>173</v>
       </c>
       <c r="B97" t="s">
         <v>150</v>
@@ -17482,7 +17482,7 @@
         <v>24</v>
       </c>
       <c r="D97">
-        <v>0.295933734939759</v>
+        <v>0.295953815261044</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -17643,7 +17643,7 @@
     </row>
     <row r="98" spans="1:56">
       <c r="A98" s="1">
-        <v>151</v>
+        <v>565</v>
       </c>
       <c r="B98" t="s">
         <v>151</v>
@@ -17813,7 +17813,7 @@
     </row>
     <row r="99" spans="1:56">
       <c r="A99" s="1">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="B99" t="s">
         <v>152</v>
@@ -17983,7 +17983,7 @@
     </row>
     <row r="100" spans="1:56">
       <c r="A100" s="1">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B100" t="s">
         <v>153</v>
@@ -17992,7 +17992,7 @@
         <v>101</v>
       </c>
       <c r="D100">
-        <v>0.295241858523202</v>
+        <v>0.295271979005129</v>
       </c>
       <c r="E100">
         <v>0</v>
@@ -18153,7 +18153,7 @@
     </row>
     <row r="101" spans="1:56">
       <c r="A101" s="1">
-        <v>379</v>
+        <v>314</v>
       </c>
       <c r="B101" t="s">
         <v>154</v>
@@ -18162,7 +18162,7 @@
         <v>41</v>
       </c>
       <c r="D101">
-        <v>0.293769712998335</v>
+        <v>0.293799833480263</v>
       </c>
       <c r="E101">
         <v>0</v>
@@ -18323,7 +18323,7 @@
     </row>
     <row r="102" spans="1:56">
       <c r="A102" s="1">
-        <v>468</v>
+        <v>60</v>
       </c>
       <c r="B102" t="s">
         <v>155</v>
@@ -18332,7 +18332,7 @@
         <v>284</v>
       </c>
       <c r="D102">
-        <v>0.293372079868771</v>
+        <v>0.293362039708128</v>
       </c>
       <c r="E102">
         <v>0</v>
@@ -18493,7 +18493,7 @@
     </row>
     <row r="103" spans="1:56">
       <c r="A103" s="1">
-        <v>644</v>
+        <v>305</v>
       </c>
       <c r="B103" t="s">
         <v>156</v>
@@ -18502,7 +18502,7 @@
         <v>65</v>
       </c>
       <c r="D103">
-        <v>0.2929046957059</v>
+        <v>0.292934816187828</v>
       </c>
       <c r="E103">
         <v>0</v>
@@ -18663,7 +18663,7 @@
     </row>
     <row r="104" spans="1:56">
       <c r="A104" s="1">
-        <v>567</v>
+        <v>309</v>
       </c>
       <c r="B104" t="s">
         <v>157</v>
@@ -18672,7 +18672,7 @@
         <v>160</v>
       </c>
       <c r="D104">
-        <v>0.292846385542169</v>
+        <v>0.292816265060241</v>
       </c>
       <c r="E104">
         <v>0</v>
@@ -18833,7 +18833,7 @@
     </row>
     <row r="105" spans="1:56">
       <c r="A105" s="1">
-        <v>401</v>
+        <v>239</v>
       </c>
       <c r="B105" t="s">
         <v>158</v>
@@ -19003,7 +19003,7 @@
     </row>
     <row r="106" spans="1:56">
       <c r="A106" s="1">
-        <v>381</v>
+        <v>106</v>
       </c>
       <c r="B106" t="s">
         <v>159</v>
@@ -19012,7 +19012,7 @@
         <v>112</v>
       </c>
       <c r="D106">
-        <v>0.290024383247275</v>
+        <v>0.29004446356856</v>
       </c>
       <c r="E106">
         <v>0</v>
@@ -19173,7 +19173,7 @@
     </row>
     <row r="107" spans="1:56">
       <c r="A107" s="1">
-        <v>28</v>
+        <v>511</v>
       </c>
       <c r="B107" t="s">
         <v>160</v>
@@ -19182,7 +19182,7 @@
         <v>140</v>
       </c>
       <c r="D107">
-        <v>0.289840791738382</v>
+        <v>0.289860872059667</v>
       </c>
       <c r="E107">
         <v>0</v>
@@ -19343,7 +19343,7 @@
     </row>
     <row r="108" spans="1:56">
       <c r="A108" s="1">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B108" t="s">
         <v>161</v>
@@ -19513,7 +19513,7 @@
     </row>
     <row r="109" spans="1:56">
       <c r="A109" s="1">
-        <v>482</v>
+        <v>57</v>
       </c>
       <c r="B109" t="s">
         <v>162</v>
@@ -19683,7 +19683,7 @@
     </row>
     <row r="110" spans="1:56">
       <c r="A110" s="1">
-        <v>574</v>
+        <v>1</v>
       </c>
       <c r="B110" t="s">
         <v>163</v>
@@ -19853,7 +19853,7 @@
     </row>
     <row r="111" spans="1:56">
       <c r="A111" s="1">
-        <v>532</v>
+        <v>31</v>
       </c>
       <c r="B111" t="s">
         <v>164</v>
@@ -19862,7 +19862,7 @@
         <v>61</v>
       </c>
       <c r="D111">
-        <v>0.284812693396537</v>
+        <v>0.28482273355718</v>
       </c>
       <c r="E111">
         <v>0</v>
@@ -20023,16 +20023,16 @@
     </row>
     <row r="112" spans="1:56">
       <c r="A112" s="1">
-        <v>98</v>
+        <v>270</v>
       </c>
       <c r="B112" t="s">
         <v>165</v>
       </c>
       <c r="C112">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="D112">
-        <v>0.280180722891566</v>
+        <v>0.280185185185185</v>
       </c>
       <c r="E112">
         <v>0</v>
@@ -20047,10 +20047,10 @@
         <v>0</v>
       </c>
       <c r="I112">
-        <v>0</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="J112">
-        <v>0</v>
+        <v>0.037037037037037</v>
       </c>
       <c r="K112">
         <v>0</v>
@@ -20059,22 +20059,22 @@
         <v>0</v>
       </c>
       <c r="M112">
-        <v>0</v>
+        <v>0.0185185185185185</v>
       </c>
       <c r="N112">
-        <v>0.210526315789474</v>
+        <v>0.037037037037037</v>
       </c>
       <c r="O112">
-        <v>0</v>
+        <v>0.0185185185185185</v>
       </c>
       <c r="P112">
-        <v>0</v>
+        <v>0.0185185185185185</v>
       </c>
       <c r="Q112">
-        <v>0.105263157894737</v>
+        <v>0</v>
       </c>
       <c r="R112">
-        <v>0</v>
+        <v>0.0185185185185185</v>
       </c>
       <c r="S112">
         <v>0</v>
@@ -20089,13 +20089,13 @@
         <v>0</v>
       </c>
       <c r="W112">
-        <v>0.368421052631579</v>
+        <v>0.203703703703704</v>
       </c>
       <c r="X112">
         <v>0</v>
       </c>
       <c r="Y112">
-        <v>0</v>
+        <v>0.0555555555555556</v>
       </c>
       <c r="Z112">
         <v>0</v>
@@ -20113,10 +20113,10 @@
         <v>0</v>
       </c>
       <c r="AE112">
-        <v>0</v>
+        <v>0.0185185185185185</v>
       </c>
       <c r="AF112">
-        <v>0</v>
+        <v>0.037037037037037</v>
       </c>
       <c r="AG112">
         <v>0</v>
@@ -20134,16 +20134,16 @@
         <v>0</v>
       </c>
       <c r="AL112">
-        <v>0</v>
+        <v>0.0740740740740741</v>
       </c>
       <c r="AM112">
         <v>0</v>
       </c>
       <c r="AN112">
-        <v>0</v>
+        <v>0.0185185185185185</v>
       </c>
       <c r="AO112">
-        <v>0.157894736842105</v>
+        <v>0.0925925925925926</v>
       </c>
       <c r="AP112">
         <v>0</v>
@@ -20152,7 +20152,7 @@
         <v>0</v>
       </c>
       <c r="AR112">
-        <v>0</v>
+        <v>0.037037037037037</v>
       </c>
       <c r="AS112">
         <v>0</v>
@@ -20164,7 +20164,7 @@
         <v>0</v>
       </c>
       <c r="AV112">
-        <v>0.0526315789473684</v>
+        <v>0.0740740740740741</v>
       </c>
       <c r="AW112">
         <v>0</v>
@@ -20173,13 +20173,13 @@
         <v>0</v>
       </c>
       <c r="AY112">
-        <v>0</v>
+        <v>0.037037037037037</v>
       </c>
       <c r="AZ112">
         <v>0</v>
       </c>
       <c r="BA112">
-        <v>0.105263157894737</v>
+        <v>0.0925925925925926</v>
       </c>
       <c r="BB112">
         <v>0</v>
@@ -20193,16 +20193,16 @@
     </row>
     <row r="113" spans="1:56">
       <c r="A113" s="1">
-        <v>172</v>
+        <v>485</v>
       </c>
       <c r="B113" t="s">
         <v>166</v>
       </c>
       <c r="C113">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="D113">
-        <v>0.2801651048639</v>
+        <v>0.280180722891566</v>
       </c>
       <c r="E113">
         <v>0</v>
@@ -20217,10 +20217,10 @@
         <v>0</v>
       </c>
       <c r="I113">
-        <v>0.111111111111111</v>
+        <v>0</v>
       </c>
       <c r="J113">
-        <v>0.037037037037037</v>
+        <v>0</v>
       </c>
       <c r="K113">
         <v>0</v>
@@ -20229,22 +20229,22 @@
         <v>0</v>
       </c>
       <c r="M113">
-        <v>0.0185185185185185</v>
+        <v>0</v>
       </c>
       <c r="N113">
-        <v>0.037037037037037</v>
+        <v>0.210526315789474</v>
       </c>
       <c r="O113">
-        <v>0.0185185185185185</v>
+        <v>0</v>
       </c>
       <c r="P113">
-        <v>0.0185185185185185</v>
+        <v>0</v>
       </c>
       <c r="Q113">
-        <v>0</v>
+        <v>0.105263157894737</v>
       </c>
       <c r="R113">
-        <v>0.0185185185185185</v>
+        <v>0</v>
       </c>
       <c r="S113">
         <v>0</v>
@@ -20259,13 +20259,13 @@
         <v>0</v>
       </c>
       <c r="W113">
-        <v>0.203703703703704</v>
+        <v>0.368421052631579</v>
       </c>
       <c r="X113">
         <v>0</v>
       </c>
       <c r="Y113">
-        <v>0.0555555555555556</v>
+        <v>0</v>
       </c>
       <c r="Z113">
         <v>0</v>
@@ -20283,10 +20283,10 @@
         <v>0</v>
       </c>
       <c r="AE113">
-        <v>0.0185185185185185</v>
+        <v>0</v>
       </c>
       <c r="AF113">
-        <v>0.037037037037037</v>
+        <v>0</v>
       </c>
       <c r="AG113">
         <v>0</v>
@@ -20304,16 +20304,16 @@
         <v>0</v>
       </c>
       <c r="AL113">
-        <v>0.0740740740740741</v>
+        <v>0</v>
       </c>
       <c r="AM113">
         <v>0</v>
       </c>
       <c r="AN113">
-        <v>0.0185185185185185</v>
+        <v>0</v>
       </c>
       <c r="AO113">
-        <v>0.0925925925925926</v>
+        <v>0.157894736842105</v>
       </c>
       <c r="AP113">
         <v>0</v>
@@ -20322,7 +20322,7 @@
         <v>0</v>
       </c>
       <c r="AR113">
-        <v>0.037037037037037</v>
+        <v>0</v>
       </c>
       <c r="AS113">
         <v>0</v>
@@ -20334,7 +20334,7 @@
         <v>0</v>
       </c>
       <c r="AV113">
-        <v>0.0740740740740741</v>
+        <v>0.0526315789473684</v>
       </c>
       <c r="AW113">
         <v>0</v>
@@ -20343,13 +20343,13 @@
         <v>0</v>
       </c>
       <c r="AY113">
-        <v>0.037037037037037</v>
+        <v>0</v>
       </c>
       <c r="AZ113">
         <v>0</v>
       </c>
       <c r="BA113">
-        <v>0.0925925925925926</v>
+        <v>0.105263157894737</v>
       </c>
       <c r="BB113">
         <v>0</v>
@@ -20363,7 +20363,7 @@
     </row>
     <row r="114" spans="1:56">
       <c r="A114" s="1">
-        <v>199</v>
+        <v>520</v>
       </c>
       <c r="B114" t="s">
         <v>167</v>
@@ -20533,7 +20533,7 @@
     </row>
     <row r="115" spans="1:56">
       <c r="A115" s="1">
-        <v>393</v>
+        <v>277</v>
       </c>
       <c r="B115" t="s">
         <v>168</v>
@@ -20703,7 +20703,7 @@
     </row>
     <row r="116" spans="1:56">
       <c r="A116" s="1">
-        <v>218</v>
+        <v>542</v>
       </c>
       <c r="B116" t="s">
         <v>169</v>
@@ -20873,7 +20873,7 @@
     </row>
     <row r="117" spans="1:56">
       <c r="A117" s="1">
-        <v>651</v>
+        <v>293</v>
       </c>
       <c r="B117" t="s">
         <v>170</v>
@@ -20882,7 +20882,7 @@
         <v>527</v>
       </c>
       <c r="D117">
-        <v>0.277788897525586</v>
+        <v>0.277798937686229</v>
       </c>
       <c r="E117">
         <v>0</v>
@@ -21043,7 +21043,7 @@
     </row>
     <row r="118" spans="1:56">
       <c r="A118" s="1">
-        <v>604</v>
+        <v>550</v>
       </c>
       <c r="B118" t="s">
         <v>171</v>
@@ -21052,7 +21052,7 @@
         <v>19</v>
       </c>
       <c r="D118">
-        <v>0.277328260410061</v>
+        <v>0.277348340731346</v>
       </c>
       <c r="E118">
         <v>0</v>
@@ -21213,7 +21213,7 @@
     </row>
     <row r="119" spans="1:56">
       <c r="A119" s="1">
-        <v>522</v>
+        <v>655</v>
       </c>
       <c r="B119" t="s">
         <v>172</v>
@@ -21222,7 +21222,7 @@
         <v>49</v>
       </c>
       <c r="D119">
-        <v>0.276921973608721</v>
+        <v>0.276932013769363</v>
       </c>
       <c r="E119">
         <v>0</v>
@@ -21383,7 +21383,7 @@
     </row>
     <row r="120" spans="1:56">
       <c r="A120" s="1">
-        <v>170</v>
+        <v>29</v>
       </c>
       <c r="B120" t="s">
         <v>173</v>
@@ -21553,7 +21553,7 @@
     </row>
     <row r="121" spans="1:56">
       <c r="A121" s="1">
-        <v>236</v>
+        <v>127</v>
       </c>
       <c r="B121" t="s">
         <v>174</v>
@@ -21562,7 +21562,7 @@
         <v>75</v>
       </c>
       <c r="D121">
-        <v>0.274568273092369</v>
+        <v>0.274558232931727</v>
       </c>
       <c r="E121">
         <v>0</v>
@@ -21723,7 +21723,7 @@
     </row>
     <row r="122" spans="1:56">
       <c r="A122" s="1">
-        <v>34</v>
+        <v>578</v>
       </c>
       <c r="B122" t="s">
         <v>175</v>
@@ -21732,7 +21732,7 @@
         <v>120</v>
       </c>
       <c r="D122">
-        <v>0.274236947791165</v>
+        <v>0.274246987951807</v>
       </c>
       <c r="E122">
         <v>0</v>
@@ -21893,7 +21893,7 @@
     </row>
     <row r="123" spans="1:56">
       <c r="A123" s="1">
-        <v>216</v>
+        <v>592</v>
       </c>
       <c r="B123" t="s">
         <v>176</v>
@@ -21902,7 +21902,7 @@
         <v>21</v>
       </c>
       <c r="D123">
-        <v>0.273475329890992</v>
+        <v>0.273495410212278</v>
       </c>
       <c r="E123">
         <v>0</v>
@@ -22063,7 +22063,7 @@
     </row>
     <row r="124" spans="1:56">
       <c r="A124" s="1">
-        <v>642</v>
+        <v>624</v>
       </c>
       <c r="B124" t="s">
         <v>177</v>
@@ -22072,7 +22072,7 @@
         <v>557</v>
       </c>
       <c r="D124">
-        <v>0.273320733562617</v>
+        <v>0.273290613080689</v>
       </c>
       <c r="E124">
         <v>0</v>
@@ -22233,7 +22233,7 @@
     </row>
     <row r="125" spans="1:56">
       <c r="A125" s="1">
-        <v>253</v>
+        <v>132</v>
       </c>
       <c r="B125" t="s">
         <v>178</v>
@@ -22403,7 +22403,7 @@
     </row>
     <row r="126" spans="1:56">
       <c r="A126" s="1">
-        <v>260</v>
+        <v>449</v>
       </c>
       <c r="B126" t="s">
         <v>179</v>
@@ -22573,7 +22573,7 @@
     </row>
     <row r="127" spans="1:56">
       <c r="A127" s="1">
-        <v>123</v>
+        <v>26</v>
       </c>
       <c r="B127" t="s">
         <v>180</v>
@@ -22743,7 +22743,7 @@
     </row>
     <row r="128" spans="1:56">
       <c r="A128" s="1">
-        <v>540</v>
+        <v>295</v>
       </c>
       <c r="B128" t="s">
         <v>181</v>
@@ -22913,7 +22913,7 @@
     </row>
     <row r="129" spans="1:56">
       <c r="A129" s="1">
-        <v>471</v>
+        <v>387</v>
       </c>
       <c r="B129" t="s">
         <v>182</v>
@@ -22922,7 +22922,7 @@
         <v>692</v>
       </c>
       <c r="D129">
-        <v>0.266269470947373</v>
+        <v>0.266279511108016</v>
       </c>
       <c r="E129">
         <v>0</v>
@@ -23083,7 +23083,7 @@
     </row>
     <row r="130" spans="1:56">
       <c r="A130" s="1">
-        <v>511</v>
+        <v>19</v>
       </c>
       <c r="B130" t="s">
         <v>183</v>
@@ -23092,7 +23092,7 @@
         <v>19</v>
       </c>
       <c r="D130">
-        <v>0.26541058972733</v>
+        <v>0.265430670048616</v>
       </c>
       <c r="E130">
         <v>0</v>
@@ -23253,7 +23253,7 @@
     </row>
     <row r="131" spans="1:56">
       <c r="A131" s="1">
-        <v>237</v>
+        <v>327</v>
       </c>
       <c r="B131" t="s">
         <v>184</v>
@@ -23262,7 +23262,7 @@
         <v>41</v>
       </c>
       <c r="D131">
-        <v>0.2642033989617</v>
+        <v>0.264223479282986</v>
       </c>
       <c r="E131">
         <v>0</v>
@@ -23423,7 +23423,7 @@
     </row>
     <row r="132" spans="1:56">
       <c r="A132" s="1">
-        <v>166</v>
+        <v>90</v>
       </c>
       <c r="B132" t="s">
         <v>185</v>
@@ -23432,7 +23432,7 @@
         <v>52</v>
       </c>
       <c r="D132">
-        <v>0.263188137164041</v>
+        <v>0.263208217485326</v>
       </c>
       <c r="E132">
         <v>0</v>
@@ -23593,7 +23593,7 @@
     </row>
     <row r="133" spans="1:56">
       <c r="A133" s="1">
-        <v>489</v>
+        <v>557</v>
       </c>
       <c r="B133" t="s">
         <v>186</v>
@@ -23602,7 +23602,7 @@
         <v>119</v>
       </c>
       <c r="D133">
-        <v>0.26288962572981</v>
+        <v>0.262919746211738</v>
       </c>
       <c r="E133">
         <v>0</v>
@@ -23763,7 +23763,7 @@
     </row>
     <row r="134" spans="1:56">
       <c r="A134" s="1">
-        <v>456</v>
+        <v>328</v>
       </c>
       <c r="B134" t="s">
         <v>187</v>
@@ -23933,7 +23933,7 @@
     </row>
     <row r="135" spans="1:56">
       <c r="A135" s="1">
-        <v>363</v>
+        <v>489</v>
       </c>
       <c r="B135" t="s">
         <v>188</v>
@@ -23942,7 +23942,7 @@
         <v>93</v>
       </c>
       <c r="D135">
-        <v>0.262583560046638</v>
+        <v>0.262563479725353</v>
       </c>
       <c r="E135">
         <v>0</v>
@@ -24103,7 +24103,7 @@
     </row>
     <row r="136" spans="1:56">
       <c r="A136" s="1">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="B136" t="s">
         <v>189</v>
@@ -24273,7 +24273,7 @@
     </row>
     <row r="137" spans="1:56">
       <c r="A137" s="1">
-        <v>627</v>
+        <v>439</v>
       </c>
       <c r="B137" t="s">
         <v>190</v>
@@ -24282,7 +24282,7 @@
         <v>179</v>
       </c>
       <c r="D137">
-        <v>0.261924457606964</v>
+        <v>0.261954578088892</v>
       </c>
       <c r="E137">
         <v>0</v>
@@ -24443,7 +24443,7 @@
     </row>
     <row r="138" spans="1:56">
       <c r="A138" s="1">
-        <v>615</v>
+        <v>76</v>
       </c>
       <c r="B138" t="s">
         <v>191</v>
@@ -24452,7 +24452,7 @@
         <v>86</v>
       </c>
       <c r="D138">
-        <v>0.261317128981041</v>
+        <v>0.26131712898104</v>
       </c>
       <c r="E138">
         <v>0</v>
@@ -24613,7 +24613,7 @@
     </row>
     <row r="139" spans="1:56">
       <c r="A139" s="1">
-        <v>347</v>
+        <v>413</v>
       </c>
       <c r="B139" t="s">
         <v>192</v>
@@ -24622,7 +24622,7 @@
         <v>146</v>
       </c>
       <c r="D139">
-        <v>0.260435027782362</v>
+        <v>0.260445067943005</v>
       </c>
       <c r="E139">
         <v>0</v>
@@ -24783,7 +24783,7 @@
     </row>
     <row r="140" spans="1:56">
       <c r="A140" s="1">
-        <v>57</v>
+        <v>666</v>
       </c>
       <c r="B140" t="s">
         <v>193</v>
@@ -24792,7 +24792,7 @@
         <v>1308</v>
       </c>
       <c r="D140">
-        <v>0.25917421981504</v>
+        <v>0.259144099333112</v>
       </c>
       <c r="E140">
         <v>0</v>
@@ -24953,7 +24953,7 @@
     </row>
     <row r="141" spans="1:56">
       <c r="A141" s="1">
-        <v>72</v>
+        <v>646</v>
       </c>
       <c r="B141" t="s">
         <v>194</v>
@@ -24962,7 +24962,7 @@
         <v>285</v>
       </c>
       <c r="D141">
-        <v>0.257438173747622</v>
+        <v>0.257418093426337</v>
       </c>
       <c r="E141">
         <v>0</v>
@@ -25123,7 +25123,7 @@
     </row>
     <row r="142" spans="1:56">
       <c r="A142" s="1">
-        <v>582</v>
+        <v>556</v>
       </c>
       <c r="B142" t="s">
         <v>195</v>
@@ -25132,7 +25132,7 @@
         <v>283</v>
       </c>
       <c r="D142">
-        <v>0.257172790100331</v>
+        <v>0.257142669618403</v>
       </c>
       <c r="E142">
         <v>0</v>
@@ -25293,7 +25293,7 @@
     </row>
     <row r="143" spans="1:56">
       <c r="A143" s="1">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="B143" t="s">
         <v>196</v>
@@ -25302,7 +25302,7 @@
         <v>442</v>
       </c>
       <c r="D143">
-        <v>0.256396536371731</v>
+        <v>0.256366415889804</v>
       </c>
       <c r="E143">
         <v>0</v>
@@ -25463,7 +25463,7 @@
     </row>
     <row r="144" spans="1:56">
       <c r="A144" s="1">
-        <v>187</v>
+        <v>347</v>
       </c>
       <c r="B144" t="s">
         <v>197</v>
@@ -25472,7 +25472,7 @@
         <v>90</v>
       </c>
       <c r="D144">
-        <v>0.255087014725569</v>
+        <v>0.255076974564926</v>
       </c>
       <c r="E144">
         <v>0</v>
@@ -25633,7 +25633,7 @@
     </row>
     <row r="145" spans="1:56">
       <c r="A145" s="1">
-        <v>122</v>
+        <v>296</v>
       </c>
       <c r="B145" t="s">
         <v>198</v>
@@ -25642,7 +25642,7 @@
         <v>117</v>
       </c>
       <c r="D145">
-        <v>0.253262537328802</v>
+        <v>0.253282617650088</v>
       </c>
       <c r="E145">
         <v>0</v>
@@ -25803,7 +25803,7 @@
     </row>
     <row r="146" spans="1:56">
       <c r="A146" s="1">
-        <v>452</v>
+        <v>214</v>
       </c>
       <c r="B146" t="s">
         <v>199</v>
@@ -25973,7 +25973,7 @@
     </row>
     <row r="147" spans="1:56">
       <c r="A147" s="1">
-        <v>27</v>
+        <v>394</v>
       </c>
       <c r="B147" t="s">
         <v>200</v>
@@ -25982,7 +25982,7 @@
         <v>36</v>
       </c>
       <c r="D147">
-        <v>0.249571619812584</v>
+        <v>0.249601740294511</v>
       </c>
       <c r="E147">
         <v>0</v>
@@ -26143,7 +26143,7 @@
     </row>
     <row r="148" spans="1:56">
       <c r="A148" s="1">
-        <v>450</v>
+        <v>187</v>
       </c>
       <c r="B148" t="s">
         <v>201</v>
@@ -26152,7 +26152,7 @@
         <v>48</v>
       </c>
       <c r="D148">
-        <v>0.249006024096386</v>
+        <v>0.249016064257028</v>
       </c>
       <c r="E148">
         <v>0</v>
@@ -26313,7 +26313,7 @@
     </row>
     <row r="149" spans="1:56">
       <c r="A149" s="1">
-        <v>329</v>
+        <v>23</v>
       </c>
       <c r="B149" t="s">
         <v>202</v>
@@ -26322,7 +26322,7 @@
         <v>336</v>
       </c>
       <c r="D149">
-        <v>0.248663224325875</v>
+        <v>0.248633103843947</v>
       </c>
       <c r="E149">
         <v>0</v>
@@ -26483,7 +26483,7 @@
     </row>
     <row r="150" spans="1:56">
       <c r="A150" s="1">
-        <v>418</v>
+        <v>515</v>
       </c>
       <c r="B150" t="s">
         <v>203</v>
@@ -26492,7 +26492,7 @@
         <v>44</v>
       </c>
       <c r="D150">
-        <v>0.247710843373494</v>
+        <v>0.247690763052209</v>
       </c>
       <c r="E150">
         <v>0</v>
@@ -26653,7 +26653,7 @@
     </row>
     <row r="151" spans="1:56">
       <c r="A151" s="1">
-        <v>274</v>
+        <v>452</v>
       </c>
       <c r="B151" t="s">
         <v>204</v>
@@ -26662,7 +26662,7 @@
         <v>45</v>
       </c>
       <c r="D151">
-        <v>0.245619143239625</v>
+        <v>0.24563922356091</v>
       </c>
       <c r="E151">
         <v>0</v>
@@ -26823,7 +26823,7 @@
     </row>
     <row r="152" spans="1:56">
       <c r="A152" s="1">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="B152" t="s">
         <v>205</v>
@@ -26832,7 +26832,7 @@
         <v>171</v>
       </c>
       <c r="D152">
-        <v>0.24413214260551</v>
+        <v>0.244162263087437</v>
       </c>
       <c r="E152">
         <v>0</v>
@@ -26993,7 +26993,7 @@
     </row>
     <row r="153" spans="1:56">
       <c r="A153" s="1">
-        <v>96</v>
+        <v>491</v>
       </c>
       <c r="B153" t="s">
         <v>206</v>
@@ -27002,7 +27002,7 @@
         <v>129</v>
       </c>
       <c r="D153">
-        <v>0.2436195946577</v>
+        <v>0.243589474175773</v>
       </c>
       <c r="E153">
         <v>0</v>
@@ -27163,7 +27163,7 @@
     </row>
     <row r="154" spans="1:56">
       <c r="A154" s="1">
-        <v>386</v>
+        <v>499</v>
       </c>
       <c r="B154" t="s">
         <v>207</v>
@@ -27172,7 +27172,7 @@
         <v>891</v>
       </c>
       <c r="D154">
-        <v>0.241995050910714</v>
+        <v>0.242025171392641</v>
       </c>
       <c r="E154">
         <v>0</v>
@@ -27333,7 +27333,7 @@
     </row>
     <row r="155" spans="1:56">
       <c r="A155" s="1">
-        <v>640</v>
+        <v>110</v>
       </c>
       <c r="B155" t="s">
         <v>208</v>
@@ -27503,7 +27503,7 @@
     </row>
     <row r="156" spans="1:56">
       <c r="A156" s="1">
-        <v>479</v>
+        <v>258</v>
       </c>
       <c r="B156" t="s">
         <v>209</v>
@@ -27512,7 +27512,7 @@
         <v>309</v>
       </c>
       <c r="D156">
-        <v>0.236190295161227</v>
+        <v>0.2361601746793</v>
       </c>
       <c r="E156">
         <v>0</v>
@@ -27673,7 +27673,7 @@
     </row>
     <row r="157" spans="1:56">
       <c r="A157" s="1">
-        <v>587</v>
+        <v>101</v>
       </c>
       <c r="B157" t="s">
         <v>210</v>
@@ -27682,7 +27682,7 @@
         <v>26</v>
       </c>
       <c r="D157">
-        <v>0.235592369477912</v>
+        <v>0.235602409638554</v>
       </c>
       <c r="E157">
         <v>0</v>
@@ -27843,7 +27843,7 @@
     </row>
     <row r="158" spans="1:56">
       <c r="A158" s="1">
-        <v>54</v>
+        <v>278</v>
       </c>
       <c r="B158" t="s">
         <v>211</v>
@@ -28013,7 +28013,7 @@
     </row>
     <row r="159" spans="1:56">
       <c r="A159" s="1">
-        <v>515</v>
+        <v>445</v>
       </c>
       <c r="B159" t="s">
         <v>212</v>
@@ -28183,7 +28183,7 @@
     </row>
     <row r="160" spans="1:56">
       <c r="A160" s="1">
-        <v>213</v>
+        <v>610</v>
       </c>
       <c r="B160" t="s">
         <v>213</v>
@@ -28192,7 +28192,7 @@
         <v>95</v>
       </c>
       <c r="D160">
-        <v>0.23349503276263</v>
+        <v>0.233484992601987</v>
       </c>
       <c r="E160">
         <v>0</v>
@@ -28353,7 +28353,7 @@
     </row>
     <row r="161" spans="1:56">
       <c r="A161" s="1">
-        <v>292</v>
+        <v>539</v>
       </c>
       <c r="B161" t="s">
         <v>214</v>
@@ -28362,7 +28362,7 @@
         <v>741</v>
       </c>
       <c r="D161">
-        <v>0.231402167373949</v>
+        <v>0.231412207534592</v>
       </c>
       <c r="E161">
         <v>0</v>
@@ -28523,7 +28523,7 @@
     </row>
     <row r="162" spans="1:56">
       <c r="A162" s="1">
-        <v>15</v>
+        <v>548</v>
       </c>
       <c r="B162" t="s">
         <v>215</v>
@@ -28532,7 +28532,7 @@
         <v>75</v>
       </c>
       <c r="D162">
-        <v>0.224277108433735</v>
+        <v>0.224287148594377</v>
       </c>
       <c r="E162">
         <v>0</v>
@@ -28693,7 +28693,7 @@
     </row>
     <row r="163" spans="1:56">
       <c r="A163" s="1">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="B163" t="s">
         <v>216</v>
@@ -28702,7 +28702,7 @@
         <v>80</v>
       </c>
       <c r="D163">
-        <v>0.223473895582329</v>
+        <v>0.223453815261044</v>
       </c>
       <c r="E163">
         <v>0</v>
@@ -28863,7 +28863,7 @@
     </row>
     <row r="164" spans="1:56">
       <c r="A164" s="1">
-        <v>365</v>
+        <v>172</v>
       </c>
       <c r="B164" t="s">
         <v>217</v>
@@ -28872,7 +28872,7 @@
         <v>144</v>
       </c>
       <c r="D164">
-        <v>0.221087684069612</v>
+        <v>0.221097724230254</v>
       </c>
       <c r="E164">
         <v>0</v>
@@ -29033,7 +29033,7 @@
     </row>
     <row r="165" spans="1:56">
       <c r="A165" s="1">
-        <v>413</v>
+        <v>625</v>
       </c>
       <c r="B165" t="s">
         <v>218</v>
@@ -29042,7 +29042,7 @@
         <v>444</v>
       </c>
       <c r="D165">
-        <v>0.220968197112775</v>
+        <v>0.220978237273418</v>
       </c>
       <c r="E165">
         <v>0</v>
@@ -29203,7 +29203,7 @@
     </row>
     <row r="166" spans="1:56">
       <c r="A166" s="1">
-        <v>475</v>
+        <v>86</v>
       </c>
       <c r="B166" t="s">
         <v>219</v>
@@ -29212,7 +29212,7 @@
         <v>321</v>
       </c>
       <c r="D166">
-        <v>0.218834684532523</v>
+        <v>0.218814604211237</v>
       </c>
       <c r="E166">
         <v>0</v>
@@ -29373,7 +29373,7 @@
     </row>
     <row r="167" spans="1:56">
       <c r="A167" s="1">
-        <v>397</v>
+        <v>116</v>
       </c>
       <c r="B167" t="s">
         <v>220</v>
@@ -29382,7 +29382,7 @@
         <v>307</v>
       </c>
       <c r="D167">
-        <v>0.218362080242795</v>
+        <v>0.218392200724723</v>
       </c>
       <c r="E167">
         <v>0</v>
@@ -29543,7 +29543,7 @@
     </row>
     <row r="168" spans="1:56">
       <c r="A168" s="1">
-        <v>142</v>
+        <v>574</v>
       </c>
       <c r="B168" t="s">
         <v>221</v>
@@ -29552,7 +29552,7 @@
         <v>300</v>
       </c>
       <c r="D168">
-        <v>0.218253012048193</v>
+        <v>0.218232931726908</v>
       </c>
       <c r="E168">
         <v>0</v>
@@ -29713,7 +29713,7 @@
     </row>
     <row r="169" spans="1:56">
       <c r="A169" s="1">
-        <v>93</v>
+        <v>381</v>
       </c>
       <c r="B169" t="s">
         <v>222</v>
@@ -29722,7 +29722,7 @@
         <v>761</v>
       </c>
       <c r="D169">
-        <v>0.217790768857295</v>
+        <v>0.217820889339223</v>
       </c>
       <c r="E169">
         <v>0</v>
@@ -29883,7 +29883,7 @@
     </row>
     <row r="170" spans="1:56">
       <c r="A170" s="1">
-        <v>207</v>
+        <v>79</v>
       </c>
       <c r="B170" t="s">
         <v>223</v>
@@ -29892,7 +29892,7 @@
         <v>208</v>
       </c>
       <c r="D170">
-        <v>0.217679950571517</v>
+        <v>0.217700030892802</v>
       </c>
       <c r="E170">
         <v>0</v>
@@ -30053,7 +30053,7 @@
     </row>
     <row r="171" spans="1:56">
       <c r="A171" s="1">
-        <v>227</v>
+        <v>482</v>
       </c>
       <c r="B171" t="s">
         <v>224</v>
@@ -30062,7 +30062,7 @@
         <v>80</v>
       </c>
       <c r="D171">
-        <v>0.216546184738956</v>
+        <v>0.216566265060241</v>
       </c>
       <c r="E171">
         <v>0</v>
@@ -30223,7 +30223,7 @@
     </row>
     <row r="172" spans="1:56">
       <c r="A172" s="1">
-        <v>446</v>
+        <v>570</v>
       </c>
       <c r="B172" t="s">
         <v>225</v>
@@ -30232,7 +30232,7 @@
         <v>27</v>
       </c>
       <c r="D172">
-        <v>0.214519187862561</v>
+        <v>0.214529228023204</v>
       </c>
       <c r="E172">
         <v>0</v>
@@ -30393,7 +30393,7 @@
     </row>
     <row r="173" spans="1:56">
       <c r="A173" s="1">
-        <v>560</v>
+        <v>317</v>
       </c>
       <c r="B173" t="s">
         <v>226</v>
@@ -30402,7 +30402,7 @@
         <v>98</v>
       </c>
       <c r="D173">
-        <v>0.212324604540611</v>
+        <v>0.212304524219326</v>
       </c>
       <c r="E173">
         <v>0</v>
@@ -30563,7 +30563,7 @@
     </row>
     <row r="174" spans="1:56">
       <c r="A174" s="1">
-        <v>383</v>
+        <v>623</v>
       </c>
       <c r="B174" t="s">
         <v>227</v>
@@ -30572,7 +30572,7 @@
         <v>53</v>
       </c>
       <c r="D174">
-        <v>0.210843373493976</v>
+        <v>0.210873493975904</v>
       </c>
       <c r="E174">
         <v>0</v>
@@ -30733,7 +30733,7 @@
     </row>
     <row r="175" spans="1:56">
       <c r="A175" s="1">
-        <v>241</v>
+        <v>616</v>
       </c>
       <c r="B175" t="s">
         <v>228</v>
@@ -30903,7 +30903,7 @@
     </row>
     <row r="176" spans="1:56">
       <c r="A176" s="1">
-        <v>272</v>
+        <v>600</v>
       </c>
       <c r="B176" t="s">
         <v>229</v>
@@ -30912,7 +30912,7 @@
         <v>121</v>
       </c>
       <c r="D176">
-        <v>0.207797304922168</v>
+        <v>0.207807345082811</v>
       </c>
       <c r="E176">
         <v>0</v>
@@ -31073,7 +31073,7 @@
     </row>
     <row r="177" spans="1:56">
       <c r="A177" s="1">
-        <v>502</v>
+        <v>95</v>
       </c>
       <c r="B177" t="s">
         <v>230</v>
@@ -31082,7 +31082,7 @@
         <v>2019</v>
       </c>
       <c r="D177">
-        <v>0.207228318922048</v>
+        <v>0.207258439403975</v>
       </c>
       <c r="E177">
         <v>0</v>
@@ -31243,7 +31243,7 @@
     </row>
     <row r="178" spans="1:56">
       <c r="A178" s="1">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B178" t="s">
         <v>231</v>
@@ -31252,7 +31252,7 @@
         <v>191</v>
       </c>
       <c r="D178">
-        <v>0.206169547299144</v>
+        <v>0.206189627620429</v>
       </c>
       <c r="E178">
         <v>0</v>
@@ -31413,7 +31413,7 @@
     </row>
     <row r="179" spans="1:56">
       <c r="A179" s="1">
-        <v>530</v>
+        <v>249</v>
       </c>
       <c r="B179" t="s">
         <v>232</v>
@@ -31422,7 +31422,7 @@
         <v>2292</v>
       </c>
       <c r="D179">
-        <v>0.205500431043546</v>
+        <v>0.205530551525474</v>
       </c>
       <c r="E179">
         <v>0</v>
@@ -31583,7 +31583,7 @@
     </row>
     <row r="180" spans="1:56">
       <c r="A180" s="1">
-        <v>606</v>
+        <v>298</v>
       </c>
       <c r="B180" t="s">
         <v>233</v>
@@ -31592,7 +31592,7 @@
         <v>107</v>
       </c>
       <c r="D180">
-        <v>0.204118436362271</v>
+        <v>0.204138516683557</v>
       </c>
       <c r="E180">
         <v>0</v>
@@ -31753,7 +31753,7 @@
     </row>
     <row r="181" spans="1:56">
       <c r="A181" s="1">
-        <v>20</v>
+        <v>373</v>
       </c>
       <c r="B181" t="s">
         <v>234</v>
@@ -31762,7 +31762,7 @@
         <v>345</v>
       </c>
       <c r="D181">
-        <v>0.203541994063209</v>
+        <v>0.203511873581282</v>
       </c>
       <c r="E181">
         <v>0</v>
@@ -31923,7 +31923,7 @@
     </row>
     <row r="182" spans="1:56">
       <c r="A182" s="1">
-        <v>87</v>
+        <v>571</v>
       </c>
       <c r="B182" t="s">
         <v>235</v>
@@ -31932,7 +31932,7 @@
         <v>82</v>
       </c>
       <c r="D182">
-        <v>0.193827505142521</v>
+        <v>0.193837545303164</v>
       </c>
       <c r="E182">
         <v>0</v>
@@ -32093,7 +32093,7 @@
     </row>
     <row r="183" spans="1:56">
       <c r="A183" s="1">
-        <v>230</v>
+        <v>513</v>
       </c>
       <c r="B183" t="s">
         <v>236</v>
@@ -32102,7 +32102,7 @@
         <v>188</v>
       </c>
       <c r="D183">
-        <v>0.193242758267111</v>
+        <v>0.193232718106468</v>
       </c>
       <c r="E183">
         <v>0</v>
@@ -32263,7 +32263,7 @@
     </row>
     <row r="184" spans="1:56">
       <c r="A184" s="1">
-        <v>101</v>
+        <v>272</v>
       </c>
       <c r="B184" t="s">
         <v>237</v>
@@ -32272,7 +32272,7 @@
         <v>331</v>
       </c>
       <c r="D184">
-        <v>0.192458474380907</v>
+        <v>0.192488594862835</v>
       </c>
       <c r="E184">
         <v>0</v>
@@ -32433,7 +32433,7 @@
     </row>
     <row r="185" spans="1:56">
       <c r="A185" s="1">
-        <v>427</v>
+        <v>372</v>
       </c>
       <c r="B185" t="s">
         <v>238</v>
@@ -32442,7 +32442,7 @@
         <v>1187</v>
       </c>
       <c r="D185">
-        <v>0.192076866860872</v>
+        <v>0.192046746378945</v>
       </c>
       <c r="E185">
         <v>0</v>
@@ -32603,7 +32603,7 @@
     </row>
     <row r="186" spans="1:56">
       <c r="A186" s="1">
-        <v>425</v>
+        <v>374</v>
       </c>
       <c r="B186" t="s">
         <v>239</v>
@@ -32612,7 +32612,7 @@
         <v>1248</v>
       </c>
       <c r="D186">
-        <v>0.191827309236948</v>
+        <v>0.19179718875502</v>
       </c>
       <c r="E186">
         <v>0</v>
@@ -32773,7 +32773,7 @@
     </row>
     <row r="187" spans="1:56">
       <c r="A187" s="1">
-        <v>428</v>
+        <v>636</v>
       </c>
       <c r="B187" t="s">
         <v>240</v>
@@ -32782,7 +32782,7 @@
         <v>36</v>
       </c>
       <c r="D187">
-        <v>0.188989290495315</v>
+        <v>0.188999330655957</v>
       </c>
       <c r="E187">
         <v>0</v>
@@ -32943,7 +32943,7 @@
     </row>
     <row r="188" spans="1:56">
       <c r="A188" s="1">
-        <v>513</v>
+        <v>545</v>
       </c>
       <c r="B188" t="s">
         <v>241</v>
@@ -32952,7 +32952,7 @@
         <v>365</v>
       </c>
       <c r="D188">
-        <v>0.188404714749409</v>
+        <v>0.188434835231336</v>
       </c>
       <c r="E188">
         <v>0</v>
@@ -33113,7 +33113,7 @@
     </row>
     <row r="189" spans="1:56">
       <c r="A189" s="1">
-        <v>434</v>
+        <v>282</v>
       </c>
       <c r="B189" t="s">
         <v>242</v>
@@ -33122,7 +33122,7 @@
         <v>1730</v>
       </c>
       <c r="D189">
-        <v>0.186195591615015</v>
+        <v>0.186165471133087</v>
       </c>
       <c r="E189">
         <v>0</v>
@@ -33283,7 +33283,7 @@
     </row>
     <row r="190" spans="1:56">
       <c r="A190" s="1">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="B190" t="s">
         <v>243</v>
@@ -33292,7 +33292,7 @@
         <v>671</v>
       </c>
       <c r="D190">
-        <v>0.185369570682132</v>
+        <v>0.185339450200205</v>
       </c>
       <c r="E190">
         <v>0</v>
@@ -33453,7 +33453,7 @@
     </row>
     <row r="191" spans="1:56">
       <c r="A191" s="1">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="B191" t="s">
         <v>244</v>
@@ -33462,7 +33462,7 @@
         <v>773</v>
       </c>
       <c r="D191">
-        <v>0.18345177605636</v>
+        <v>0.183421655574432</v>
       </c>
       <c r="E191">
         <v>0</v>
@@ -33623,7 +33623,7 @@
     </row>
     <row r="192" spans="1:56">
       <c r="A192" s="1">
-        <v>266</v>
+        <v>165</v>
       </c>
       <c r="B192" t="s">
         <v>245</v>
@@ -33632,7 +33632,7 @@
         <v>488</v>
       </c>
       <c r="D192">
-        <v>0.167544275462506</v>
+        <v>0.167554315623148</v>
       </c>
       <c r="E192">
         <v>0</v>
@@ -33793,7 +33793,7 @@
     </row>
     <row r="193" spans="1:56">
       <c r="A193" s="1">
-        <v>301</v>
+        <v>342</v>
       </c>
       <c r="B193" t="s">
         <v>246</v>
@@ -33802,7 +33802,7 @@
         <v>466</v>
       </c>
       <c r="D193">
-        <v>0.159888954961477</v>
+        <v>0.159858834479549</v>
       </c>
       <c r="E193">
         <v>0</v>
@@ -33963,19 +33963,19 @@
     </row>
     <row r="194" spans="1:56">
       <c r="A194" s="1">
-        <v>43</v>
+        <v>194</v>
       </c>
       <c r="B194" t="s">
         <v>247</v>
       </c>
       <c r="C194">
-        <v>1083</v>
+        <v>162</v>
       </c>
       <c r="D194">
-        <v>0.156176117211227</v>
+        <v>0.156188457533839</v>
       </c>
       <c r="E194">
-        <v>0.00277008310249307</v>
+        <v>0</v>
       </c>
       <c r="F194">
         <v>0</v>
@@ -33984,67 +33984,67 @@
         <v>0</v>
       </c>
       <c r="H194">
-        <v>0.00369344413665743</v>
+        <v>0</v>
       </c>
       <c r="I194">
-        <v>0.0193905817174515</v>
+        <v>0.0246913580246914</v>
       </c>
       <c r="J194">
-        <v>0.0193905817174515</v>
+        <v>0.0246913580246914</v>
       </c>
       <c r="K194">
-        <v>0.00831024930747922</v>
+        <v>0.00617283950617284</v>
       </c>
       <c r="L194">
-        <v>0.00646352723915051</v>
+        <v>0</v>
       </c>
       <c r="M194">
-        <v>0.0166204986149584</v>
+        <v>0.0123456790123457</v>
       </c>
       <c r="N194">
-        <v>0.0692520775623269</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="O194">
         <v>0</v>
       </c>
       <c r="P194">
-        <v>0.00923361034164358</v>
+        <v>0.0246913580246914</v>
       </c>
       <c r="Q194">
-        <v>0.120960295475531</v>
+        <v>0.104938271604938</v>
       </c>
       <c r="R194">
         <v>0</v>
       </c>
       <c r="S194">
-        <v>0.00461680517082179</v>
+        <v>0</v>
       </c>
       <c r="T194">
         <v>0</v>
       </c>
       <c r="U194">
-        <v>0.0313942751615882</v>
+        <v>0.037037037037037</v>
       </c>
       <c r="V194">
-        <v>0.00461680517082179</v>
+        <v>0</v>
       </c>
       <c r="W194">
-        <v>0.0332409972299169</v>
+        <v>0.037037037037037</v>
       </c>
       <c r="X194">
-        <v>0.00277008310249307</v>
+        <v>0.0123456790123457</v>
       </c>
       <c r="Y194">
-        <v>0.0406278855032318</v>
+        <v>0.0246913580246914</v>
       </c>
       <c r="Z194">
-        <v>0.0480147737765466</v>
+        <v>0.037037037037037</v>
       </c>
       <c r="AA194">
-        <v>0.0590951061865189</v>
+        <v>0.0432098765432099</v>
       </c>
       <c r="AB194">
-        <v>0.00738688827331487</v>
+        <v>0.00617283950617284</v>
       </c>
       <c r="AC194">
         <v>0</v>
@@ -34053,19 +34053,19 @@
         <v>0</v>
       </c>
       <c r="AE194">
-        <v>0.00369344413665743</v>
+        <v>0</v>
       </c>
       <c r="AF194">
-        <v>0.0110803324099723</v>
+        <v>0.037037037037037</v>
       </c>
       <c r="AG194">
-        <v>0.00369344413665743</v>
+        <v>0</v>
       </c>
       <c r="AH194">
         <v>0</v>
       </c>
       <c r="AI194">
-        <v>0.0212373037857802</v>
+        <v>0.037037037037037</v>
       </c>
       <c r="AJ194">
         <v>0</v>
@@ -34074,52 +34074,52 @@
         <v>0</v>
       </c>
       <c r="AL194">
-        <v>0.0470914127423823</v>
+        <v>0.0308641975308642</v>
       </c>
       <c r="AM194">
-        <v>0.00277008310249307</v>
+        <v>0</v>
       </c>
       <c r="AN194">
-        <v>0.0184672206832872</v>
+        <v>0.0185185185185185</v>
       </c>
       <c r="AO194">
-        <v>0.148661126500462</v>
+        <v>0.12962962962963</v>
       </c>
       <c r="AP194">
-        <v>0.0193905817174515</v>
+        <v>0.0246913580246914</v>
       </c>
       <c r="AQ194">
-        <v>0.0138504155124654</v>
+        <v>0.0308641975308642</v>
       </c>
       <c r="AR194">
-        <v>0.00923361034164358</v>
+        <v>0.0123456790123457</v>
       </c>
       <c r="AS194">
-        <v>0.00554016620498615</v>
+        <v>0</v>
       </c>
       <c r="AT194">
         <v>0</v>
       </c>
       <c r="AU194">
-        <v>0.00184672206832872</v>
+        <v>0</v>
       </c>
       <c r="AV194">
-        <v>0.0193905817174515</v>
+        <v>0.0246913580246914</v>
       </c>
       <c r="AW194">
-        <v>0.0147737765466297</v>
+        <v>0.0308641975308642</v>
       </c>
       <c r="AX194">
         <v>0</v>
       </c>
       <c r="AY194">
-        <v>0.012927054478301</v>
+        <v>0.0246913580246914</v>
       </c>
       <c r="AZ194">
-        <v>0.0147737765466297</v>
+        <v>0.00617283950617284</v>
       </c>
       <c r="BA194">
-        <v>0.123730378578024</v>
+        <v>0.0864197530864197</v>
       </c>
       <c r="BB194">
         <v>0</v>
@@ -34133,19 +34133,19 @@
     </row>
     <row r="195" spans="1:56">
       <c r="A195" s="1">
-        <v>202</v>
+        <v>20</v>
       </c>
       <c r="B195" t="s">
         <v>248</v>
       </c>
       <c r="C195">
-        <v>162</v>
+        <v>1083</v>
       </c>
       <c r="D195">
-        <v>0.156168377212554</v>
+        <v>0.156145996729299</v>
       </c>
       <c r="E195">
-        <v>0</v>
+        <v>0.00277008310249307</v>
       </c>
       <c r="F195">
         <v>0</v>
@@ -34154,67 +34154,67 @@
         <v>0</v>
       </c>
       <c r="H195">
-        <v>0</v>
+        <v>0.00369344413665743</v>
       </c>
       <c r="I195">
-        <v>0.0246913580246914</v>
+        <v>0.0193905817174515</v>
       </c>
       <c r="J195">
-        <v>0.0246913580246914</v>
+        <v>0.0193905817174515</v>
       </c>
       <c r="K195">
-        <v>0.00617283950617284</v>
+        <v>0.00831024930747922</v>
       </c>
       <c r="L195">
-        <v>0</v>
+        <v>0.00646352723915051</v>
       </c>
       <c r="M195">
-        <v>0.0123456790123457</v>
+        <v>0.0166204986149584</v>
       </c>
       <c r="N195">
-        <v>0.111111111111111</v>
+        <v>0.0692520775623269</v>
       </c>
       <c r="O195">
         <v>0</v>
       </c>
       <c r="P195">
-        <v>0.0246913580246914</v>
+        <v>0.00923361034164358</v>
       </c>
       <c r="Q195">
-        <v>0.104938271604938</v>
+        <v>0.120960295475531</v>
       </c>
       <c r="R195">
         <v>0</v>
       </c>
       <c r="S195">
-        <v>0</v>
+        <v>0.00461680517082179</v>
       </c>
       <c r="T195">
         <v>0</v>
       </c>
       <c r="U195">
-        <v>0.037037037037037</v>
+        <v>0.0313942751615882</v>
       </c>
       <c r="V195">
-        <v>0</v>
+        <v>0.00461680517082179</v>
       </c>
       <c r="W195">
-        <v>0.037037037037037</v>
+        <v>0.0332409972299169</v>
       </c>
       <c r="X195">
-        <v>0.0123456790123457</v>
+        <v>0.00277008310249307</v>
       </c>
       <c r="Y195">
-        <v>0.0246913580246914</v>
+        <v>0.0406278855032318</v>
       </c>
       <c r="Z195">
-        <v>0.037037037037037</v>
+        <v>0.0480147737765466</v>
       </c>
       <c r="AA195">
-        <v>0.0432098765432099</v>
+        <v>0.0590951061865189</v>
       </c>
       <c r="AB195">
-        <v>0.00617283950617284</v>
+        <v>0.00738688827331487</v>
       </c>
       <c r="AC195">
         <v>0</v>
@@ -34223,19 +34223,19 @@
         <v>0</v>
       </c>
       <c r="AE195">
-        <v>0</v>
+        <v>0.00369344413665743</v>
       </c>
       <c r="AF195">
-        <v>0.037037037037037</v>
+        <v>0.0110803324099723</v>
       </c>
       <c r="AG195">
-        <v>0</v>
+        <v>0.00369344413665743</v>
       </c>
       <c r="AH195">
         <v>0</v>
       </c>
       <c r="AI195">
-        <v>0.037037037037037</v>
+        <v>0.0212373037857802</v>
       </c>
       <c r="AJ195">
         <v>0</v>
@@ -34244,52 +34244,52 @@
         <v>0</v>
       </c>
       <c r="AL195">
-        <v>0.0308641975308642</v>
+        <v>0.0470914127423823</v>
       </c>
       <c r="AM195">
-        <v>0</v>
+        <v>0.00277008310249307</v>
       </c>
       <c r="AN195">
-        <v>0.0185185185185185</v>
+        <v>0.0184672206832872</v>
       </c>
       <c r="AO195">
-        <v>0.12962962962963</v>
+        <v>0.148661126500462</v>
       </c>
       <c r="AP195">
-        <v>0.0246913580246914</v>
+        <v>0.0193905817174515</v>
       </c>
       <c r="AQ195">
-        <v>0.0308641975308642</v>
+        <v>0.0138504155124654</v>
       </c>
       <c r="AR195">
-        <v>0.0123456790123457</v>
+        <v>0.00923361034164358</v>
       </c>
       <c r="AS195">
-        <v>0</v>
+        <v>0.00554016620498615</v>
       </c>
       <c r="AT195">
         <v>0</v>
       </c>
       <c r="AU195">
-        <v>0</v>
+        <v>0.00184672206832872</v>
       </c>
       <c r="AV195">
-        <v>0.0246913580246914</v>
+        <v>0.0193905817174515</v>
       </c>
       <c r="AW195">
-        <v>0.0308641975308642</v>
+        <v>0.0147737765466297</v>
       </c>
       <c r="AX195">
         <v>0</v>
       </c>
       <c r="AY195">
-        <v>0.0246913580246914</v>
+        <v>0.012927054478301</v>
       </c>
       <c r="AZ195">
-        <v>0.00617283950617284</v>
+        <v>0.0147737765466297</v>
       </c>
       <c r="BA195">
-        <v>0.0864197530864197</v>
+        <v>0.123730378578024</v>
       </c>
       <c r="BB195">
         <v>0</v>
@@ -34303,7 +34303,7 @@
     </row>
     <row r="196" spans="1:56">
       <c r="A196" s="1">
-        <v>346</v>
+        <v>382</v>
       </c>
       <c r="B196" t="s">
         <v>249</v>
@@ -34312,7 +34312,7 @@
         <v>721</v>
       </c>
       <c r="D196">
-        <v>0.154984403633953</v>
+        <v>0.154954283152026</v>
       </c>
       <c r="E196">
         <v>0.0013869625520111</v>
@@ -34473,7 +34473,7 @@
     </row>
     <row r="197" spans="1:56">
       <c r="A197" s="1">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B197" t="s">
         <v>250</v>
@@ -34643,7 +34643,7 @@
     </row>
     <row r="198" spans="1:56">
       <c r="A198" s="1">
-        <v>578</v>
+        <v>446</v>
       </c>
       <c r="B198" t="s">
         <v>251</v>
@@ -34652,7 +34652,7 @@
         <v>1633</v>
       </c>
       <c r="D198">
-        <v>0.134884996200356</v>
+        <v>0.134854875718428</v>
       </c>
       <c r="E198">
         <v>0.000612369871402327</v>
@@ -34813,7 +34813,7 @@
     </row>
     <row r="199" spans="1:56">
       <c r="A199" s="1">
-        <v>484</v>
+        <v>246</v>
       </c>
       <c r="B199" t="s">
         <v>252</v>
@@ -34822,7 +34822,7 @@
         <v>606</v>
       </c>
       <c r="D199">
-        <v>0.134731897888584</v>
+        <v>0.134701777406656</v>
       </c>
       <c r="E199">
         <v>0</v>
@@ -34983,7 +34983,7 @@
     </row>
     <row r="200" spans="1:56">
       <c r="A200" s="1">
-        <v>169</v>
+        <v>507</v>
       </c>
       <c r="B200" t="s">
         <v>253</v>
@@ -34992,7 +34992,7 @@
         <v>615</v>
       </c>
       <c r="D200">
-        <v>0.125402096189637</v>
+        <v>0.125387158389656</v>
       </c>
       <c r="E200">
         <v>0</v>
@@ -35153,7 +35153,7 @@
     </row>
     <row r="201" spans="1:56">
       <c r="A201" s="1">
-        <v>342</v>
+        <v>300</v>
       </c>
       <c r="B201" t="s">
         <v>254</v>
@@ -35162,7 +35162,7 @@
         <v>1333</v>
       </c>
       <c r="D201">
-        <v>0.124511572170151</v>
+        <v>0.124521612330794</v>
       </c>
       <c r="E201">
         <v>0</v>
@@ -35323,7 +35323,7 @@
     </row>
     <row r="202" spans="1:56">
       <c r="A202" s="1">
-        <v>88</v>
+        <v>498</v>
       </c>
       <c r="B202" t="s">
         <v>255</v>
@@ -35332,7 +35332,7 @@
         <v>1946</v>
       </c>
       <c r="D202">
-        <v>0.11988131353781</v>
+        <v>0.119891353698453</v>
       </c>
       <c r="E202">
         <v>0</v>
@@ -35493,7 +35493,7 @@
     </row>
     <row r="203" spans="1:56">
       <c r="A203" s="1">
-        <v>233</v>
+        <v>185</v>
       </c>
       <c r="B203" t="s">
         <v>256</v>
@@ -35502,7 +35502,7 @@
         <v>1600</v>
       </c>
       <c r="D203">
-        <v>0.111064257028112</v>
+        <v>0.111034136546185</v>
       </c>
       <c r="E203">
         <v>0.000625</v>
@@ -35663,7 +35663,7 @@
     </row>
     <row r="204" spans="1:56">
       <c r="A204" s="1">
-        <v>281</v>
+        <v>470</v>
       </c>
       <c r="B204" t="s">
         <v>257</v>
@@ -35672,7 +35672,7 @@
         <v>2079</v>
       </c>
       <c r="D204">
-        <v>0.0917287476022416</v>
+        <v>0.0916986271203139</v>
       </c>
       <c r="E204">
         <v>0</v>
@@ -35833,7 +35833,7 @@
     </row>
     <row r="205" spans="1:56">
       <c r="A205" s="1">
-        <v>518</v>
+        <v>311</v>
       </c>
       <c r="B205" t="s">
         <v>258</v>
@@ -35842,7 +35842,7 @@
         <v>2924</v>
       </c>
       <c r="D205">
-        <v>0.0811040880347656</v>
+        <v>0.0810739675528379</v>
       </c>
       <c r="E205">
         <v>0.000683994528043776</v>

</xml_diff>